<commit_message>
Correct spiderer.sage(), add IDs springer, start runall
</commit_message>
<xml_diff>
--- a/journals/springer.xlsx
+++ b/journals/springer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\projects\contentmine\journal-spider\springer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\projects\contentmine\journal-spider\journals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="260">
   <si>
     <t>subject</t>
   </si>
@@ -798,6 +798,9 @@
   </si>
   <si>
     <t>publ</t>
+  </si>
+  <si>
+    <t>springer</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1166,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E274"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,6 +1195,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>40750</v>
+      </c>
+      <c r="C2" t="s">
+        <v>259</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1200,6 +1209,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>13722</v>
+      </c>
+      <c r="C3" t="s">
+        <v>259</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1208,6 +1223,12 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>10488</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1216,6 +1237,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>40894</v>
+      </c>
+      <c r="C5" t="s">
+        <v>259</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1224,6 +1251,12 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>10461</v>
+      </c>
+      <c r="C6" t="s">
+        <v>259</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1232,6 +1265,12 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>10464</v>
+      </c>
+      <c r="C7" t="s">
+        <v>259</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1240,6 +1279,12 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>10465</v>
+      </c>
+      <c r="C8" t="s">
+        <v>259</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1248,6 +1293,12 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>40616</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1256,6 +1307,12 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>10071</v>
+      </c>
+      <c r="C10" t="s">
+        <v>259</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1264,6 +1321,12 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>12160</v>
+      </c>
+      <c r="C11" t="s">
+        <v>259</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1272,6 +1335,12 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10484</v>
+      </c>
+      <c r="C12" t="s">
+        <v>259</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1280,6 +1349,12 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10508</v>
+      </c>
+      <c r="C13" t="s">
+        <v>259</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1288,6 +1363,12 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>40405</v>
+      </c>
+      <c r="C14" t="s">
+        <v>259</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1296,6 +1377,12 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>13414</v>
+      </c>
+      <c r="C15" t="s">
+        <v>259</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1304,6 +1391,12 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>41133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>259</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1311,7 +1404,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>10516</v>
+      </c>
+      <c r="C17" t="s">
+        <v>259</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1319,7 +1418,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>40617</v>
+      </c>
+      <c r="C18" t="s">
+        <v>259</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1327,7 +1432,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>40614</v>
+      </c>
+      <c r="C19" t="s">
+        <v>259</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
@@ -1335,7 +1446,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>10519</v>
+      </c>
+      <c r="C20" t="s">
+        <v>259</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1343,7 +1460,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>13428</v>
+      </c>
+      <c r="C21" t="s">
+        <v>259</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>31</v>
       </c>
@@ -1351,7 +1474,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>13752</v>
+      </c>
+      <c r="C22" t="s">
+        <v>259</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1359,7 +1488,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>13587</v>
+      </c>
+      <c r="C23" t="s">
+        <v>259</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>33</v>
       </c>
@@ -1367,7 +1502,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>13030</v>
+      </c>
+      <c r="C24" t="s">
+        <v>259</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
@@ -1375,7 +1516,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>12304</v>
+      </c>
+      <c r="C25" t="s">
+        <v>259</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>35</v>
       </c>
@@ -1383,7 +1530,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>40359</v>
+      </c>
+      <c r="C26" t="s">
+        <v>259</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>36</v>
       </c>
@@ -1391,7 +1544,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>11682</v>
+      </c>
+      <c r="C27" t="s">
+        <v>259</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
@@ -1399,7 +1558,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>40708</v>
+      </c>
+      <c r="C28" t="s">
+        <v>259</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1407,7 +1572,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>40631</v>
+      </c>
+      <c r="C29" t="s">
+        <v>259</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>39</v>
       </c>
@@ -1415,7 +1586,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>10566</v>
+      </c>
+      <c r="C30" t="s">
+        <v>259</v>
+      </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
@@ -1423,7 +1600,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>13034</v>
+      </c>
+      <c r="C31" t="s">
+        <v>259</v>
+      </c>
       <c r="D31" s="2" t="s">
         <v>40</v>
       </c>
@@ -1431,7 +1614,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>10560</v>
+      </c>
+      <c r="C32" t="s">
+        <v>259</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>41</v>
       </c>
@@ -1439,7 +1628,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>12187</v>
+      </c>
+      <c r="C33" t="s">
+        <v>259</v>
+      </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1447,7 +1642,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>10578</v>
+      </c>
+      <c r="C34" t="s">
+        <v>259</v>
+      </c>
       <c r="D34" s="2" t="s">
         <v>7</v>
       </c>
@@ -1455,7 +1656,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>10567</v>
+      </c>
+      <c r="C35" t="s">
+        <v>259</v>
+      </c>
       <c r="D35" s="2" t="s">
         <v>8</v>
       </c>
@@ -1463,7 +1670,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>10615</v>
+      </c>
+      <c r="C36" t="s">
+        <v>259</v>
+      </c>
       <c r="D36" s="2" t="s">
         <v>42</v>
       </c>
@@ -1471,7 +1684,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>10111</v>
+      </c>
+      <c r="C37" t="s">
+        <v>259</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>43</v>
       </c>
@@ -1479,7 +1698,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>11571</v>
+      </c>
+      <c r="C38" t="s">
+        <v>259</v>
+      </c>
       <c r="D38" s="2" t="s">
         <v>44</v>
       </c>
@@ -1487,7 +1712,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>10608</v>
+      </c>
+      <c r="C39" t="s">
+        <v>259</v>
+      </c>
       <c r="D39" s="2" t="s">
         <v>45</v>
       </c>
@@ -1495,7 +1726,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>13415</v>
+      </c>
+      <c r="C40" t="s">
+        <v>259</v>
+      </c>
       <c r="D40" s="2" t="s">
         <v>46</v>
       </c>
@@ -1503,7 +1740,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>10597</v>
+      </c>
+      <c r="C41" t="s">
+        <v>259</v>
+      </c>
       <c r="D41" s="2" t="s">
         <v>47</v>
       </c>
@@ -1511,7 +1754,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>10606</v>
+      </c>
+      <c r="C42" t="s">
+        <v>259</v>
+      </c>
       <c r="D42" s="2" t="s">
         <v>48</v>
       </c>
@@ -1519,7 +1768,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>10591</v>
+      </c>
+      <c r="C43" t="s">
+        <v>259</v>
+      </c>
       <c r="D43" s="3" t="s">
         <v>49</v>
       </c>
@@ -1527,7 +1782,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>40688</v>
+      </c>
+      <c r="C44" t="s">
+        <v>259</v>
+      </c>
       <c r="D44" s="3" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1796,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>40163</v>
+      </c>
+      <c r="C45" t="s">
+        <v>259</v>
+      </c>
       <c r="D45" s="3" t="s">
         <v>50</v>
       </c>
@@ -1543,7 +1810,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>40167</v>
+      </c>
+      <c r="C46" t="s">
+        <v>259</v>
+      </c>
       <c r="D46" s="3" t="s">
         <v>51</v>
       </c>
@@ -1551,7 +1824,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>11013</v>
+      </c>
+      <c r="C47" t="s">
+        <v>259</v>
+      </c>
       <c r="D47" s="3" t="s">
         <v>52</v>
       </c>
@@ -1559,7 +1838,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>12144</v>
+      </c>
+      <c r="C48" t="s">
+        <v>259</v>
+      </c>
       <c r="D48" s="3" t="s">
         <v>53</v>
       </c>
@@ -1567,7 +1852,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>10648</v>
+      </c>
+      <c r="C49" t="s">
+        <v>259</v>
+      </c>
       <c r="D49" s="3" t="s">
         <v>10</v>
       </c>
@@ -1575,7 +1866,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>13315</v>
+      </c>
+      <c r="C50" t="s">
+        <v>259</v>
+      </c>
       <c r="D50" s="3" t="s">
         <v>54</v>
       </c>
@@ -1583,7 +1880,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>10433</v>
+      </c>
+      <c r="C51" t="s">
+        <v>259</v>
+      </c>
       <c r="D51" s="3" t="s">
         <v>55</v>
       </c>
@@ -1591,7 +1894,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>10212</v>
+      </c>
+      <c r="C52" t="s">
+        <v>259</v>
+      </c>
       <c r="D52" s="3" t="s">
         <v>11</v>
       </c>
@@ -1599,7 +1908,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>40806</v>
+      </c>
+      <c r="C53" t="s">
+        <v>259</v>
+      </c>
       <c r="D53" s="3" t="s">
         <v>56</v>
       </c>
@@ -1607,7 +1922,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>13411</v>
+      </c>
+      <c r="C54" t="s">
+        <v>259</v>
+      </c>
       <c r="D54" s="3" t="s">
         <v>57</v>
       </c>
@@ -1615,7 +1936,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>12147</v>
+      </c>
+      <c r="C55" t="s">
+        <v>259</v>
+      </c>
       <c r="D55" s="3" t="s">
         <v>58</v>
       </c>
@@ -1623,7 +1950,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>40609</v>
+      </c>
+      <c r="C56" t="s">
+        <v>259</v>
+      </c>
       <c r="D56" s="3" t="s">
         <v>59</v>
       </c>
@@ -1631,7 +1964,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>12954</v>
+      </c>
+      <c r="C57" t="s">
+        <v>259</v>
+      </c>
       <c r="D57" s="3" t="s">
         <v>60</v>
       </c>
@@ -1639,7 +1978,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>40352</v>
+      </c>
+      <c r="C58" t="s">
+        <v>259</v>
+      </c>
       <c r="D58" s="3" t="s">
         <v>61</v>
       </c>
@@ -1647,7 +1992,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>12110</v>
+      </c>
+      <c r="C59" t="s">
+        <v>259</v>
+      </c>
       <c r="D59" s="3" t="s">
         <v>62</v>
       </c>
@@ -1655,7 +2006,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>11251</v>
+      </c>
+      <c r="C60" t="s">
+        <v>259</v>
+      </c>
       <c r="D60" s="3" t="s">
         <v>12</v>
       </c>
@@ -1663,7 +2020,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>12124</v>
+      </c>
+      <c r="C61" t="s">
+        <v>259</v>
+      </c>
       <c r="D61" s="3" t="s">
         <v>63</v>
       </c>
@@ -1671,7 +2034,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>10447</v>
+      </c>
+      <c r="C62" t="s">
+        <v>259</v>
+      </c>
       <c r="D62" s="3" t="s">
         <v>64</v>
       </c>
@@ -1679,7 +2048,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>41042</v>
+      </c>
+      <c r="C63" t="s">
+        <v>259</v>
+      </c>
       <c r="D63" s="3" t="s">
         <v>65</v>
       </c>
@@ -1687,7 +2062,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>12529</v>
+      </c>
+      <c r="C64" t="s">
+        <v>259</v>
+      </c>
       <c r="D64" s="3" t="s">
         <v>66</v>
       </c>
@@ -1695,7 +2076,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>40345</v>
+      </c>
+      <c r="C65" t="s">
+        <v>259</v>
+      </c>
       <c r="D65" s="3" t="s">
         <v>67</v>
       </c>
@@ -1703,7 +2090,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>11412</v>
+      </c>
+      <c r="C66" t="s">
+        <v>259</v>
+      </c>
       <c r="D66" s="3" t="s">
         <v>68</v>
       </c>
@@ -1711,7 +2104,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>11469</v>
+      </c>
+      <c r="C67" t="s">
+        <v>259</v>
+      </c>
       <c r="D67" s="3" t="s">
         <v>69</v>
       </c>
@@ -1719,7 +2118,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>13033</v>
+      </c>
+      <c r="C68" t="s">
+        <v>259</v>
+      </c>
       <c r="D68" s="3" t="s">
         <v>70</v>
       </c>
@@ -1727,7 +2132,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>10767</v>
+      </c>
+      <c r="C69" t="s">
+        <v>259</v>
+      </c>
       <c r="D69" s="3" t="s">
         <v>71</v>
       </c>
@@ -1735,7 +2146,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>10771</v>
+      </c>
+      <c r="C70" t="s">
+        <v>259</v>
+      </c>
       <c r="D70" s="3" t="s">
         <v>72</v>
       </c>
@@ -1743,7 +2160,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>10802</v>
+      </c>
+      <c r="C71" t="s">
+        <v>259</v>
+      </c>
       <c r="D71" s="3" t="s">
         <v>73</v>
       </c>
@@ -1751,7 +2174,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>10804</v>
+      </c>
+      <c r="C72" t="s">
+        <v>259</v>
+      </c>
       <c r="D72" s="3" t="s">
         <v>74</v>
       </c>
@@ -1759,7 +2188,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>10803</v>
+      </c>
+      <c r="C73" t="s">
+        <v>259</v>
+      </c>
       <c r="D73" s="3" t="s">
         <v>75</v>
       </c>
@@ -1767,7 +2202,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>10864</v>
+      </c>
+      <c r="C74" t="s">
+        <v>259</v>
+      </c>
       <c r="D74" s="3" t="s">
         <v>76</v>
       </c>
@@ -1775,7 +2216,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>11414</v>
+      </c>
+      <c r="C75" t="s">
+        <v>259</v>
+      </c>
       <c r="D75" s="3" t="s">
         <v>77</v>
       </c>
@@ -1783,7 +2230,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>10865</v>
+      </c>
+      <c r="C76" t="s">
+        <v>259</v>
+      </c>
       <c r="D76" s="3" t="s">
         <v>78</v>
       </c>
@@ -1791,7 +2244,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>10869</v>
+      </c>
+      <c r="C77" t="s">
+        <v>259</v>
+      </c>
       <c r="D77" s="3" t="s">
         <v>79</v>
       </c>
@@ -1799,7 +2258,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>40653</v>
+      </c>
+      <c r="C78" t="s">
+        <v>259</v>
+      </c>
       <c r="D78" s="3" t="s">
         <v>80</v>
       </c>
@@ -1807,7 +2272,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>10826</v>
+      </c>
+      <c r="C79" t="s">
+        <v>259</v>
+      </c>
       <c r="D79" s="3" t="s">
         <v>81</v>
       </c>
@@ -1815,7 +2286,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>357</v>
+      </c>
+      <c r="C80" t="s">
+        <v>259</v>
+      </c>
       <c r="D80" s="3" t="s">
         <v>82</v>
       </c>
@@ -1823,7 +2300,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>10880</v>
+      </c>
+      <c r="C81" t="s">
+        <v>259</v>
+      </c>
       <c r="D81" s="3" t="s">
         <v>83</v>
       </c>
@@ -1831,7 +2314,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>10900</v>
+      </c>
+      <c r="C82" t="s">
+        <v>259</v>
+      </c>
       <c r="D82" s="3" t="s">
         <v>84</v>
       </c>
@@ -1839,7 +2328,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>10879</v>
+      </c>
+      <c r="C83" t="s">
+        <v>259</v>
+      </c>
       <c r="D83" s="3" t="s">
         <v>85</v>
       </c>
@@ -1847,7 +2342,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>40865</v>
+      </c>
+      <c r="C84" t="s">
+        <v>259</v>
+      </c>
       <c r="D84" s="3" t="s">
         <v>86</v>
       </c>
@@ -1855,7 +2356,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>10882</v>
+      </c>
+      <c r="C85" t="s">
+        <v>259</v>
+      </c>
       <c r="D85" s="3" t="s">
         <v>87</v>
       </c>
@@ -1863,7 +2370,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>10834</v>
+      </c>
+      <c r="C86" t="s">
+        <v>259</v>
+      </c>
       <c r="D86" s="3" t="s">
         <v>88</v>
       </c>
@@ -1871,7 +2384,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>10896</v>
+      </c>
+      <c r="C87" t="s">
+        <v>259</v>
+      </c>
       <c r="D87" s="3" t="s">
         <v>89</v>
       </c>
@@ -1879,7 +2398,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>10899</v>
+      </c>
+      <c r="C88" t="s">
+        <v>259</v>
+      </c>
       <c r="D88" s="3" t="s">
         <v>90</v>
       </c>
@@ -1887,7 +2412,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>10897</v>
+      </c>
+      <c r="C89" t="s">
+        <v>259</v>
+      </c>
       <c r="D89" s="3" t="s">
         <v>91</v>
       </c>
@@ -1895,7 +2426,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>10902</v>
+      </c>
+      <c r="C90" t="s">
+        <v>259</v>
+      </c>
       <c r="D90" s="3" t="s">
         <v>92</v>
       </c>
@@ -1903,7 +2440,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>40166</v>
+      </c>
+      <c r="C91" t="s">
+        <v>259</v>
+      </c>
       <c r="D91" s="3" t="s">
         <v>93</v>
       </c>
@@ -1911,7 +2454,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>10919</v>
+      </c>
+      <c r="C92" t="s">
+        <v>259</v>
+      </c>
       <c r="D92" s="3" t="s">
         <v>94</v>
       </c>
@@ -1919,7 +2468,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>10926</v>
+      </c>
+      <c r="C93" t="s">
+        <v>259</v>
+      </c>
       <c r="D93" s="3" t="s">
         <v>95</v>
       </c>
@@ -1927,7 +2482,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>40817</v>
+      </c>
+      <c r="C94" t="s">
+        <v>259</v>
+      </c>
       <c r="D94" s="3" t="s">
         <v>96</v>
       </c>
@@ -1935,7 +2496,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>11896</v>
+      </c>
+      <c r="C95" t="s">
+        <v>259</v>
+      </c>
       <c r="D95" s="3" t="s">
         <v>97</v>
       </c>
@@ -1943,7 +2510,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>10935</v>
+      </c>
+      <c r="C96" t="s">
+        <v>259</v>
+      </c>
       <c r="D96" s="3" t="s">
         <v>98</v>
       </c>
@@ -1951,7 +2524,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>10936</v>
+      </c>
+      <c r="C97" t="s">
+        <v>259</v>
+      </c>
       <c r="D97" s="3" t="s">
         <v>99</v>
       </c>
@@ -1959,7 +2538,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>10862</v>
+      </c>
+      <c r="C98" t="s">
+        <v>259</v>
+      </c>
       <c r="D98" s="3" t="s">
         <v>100</v>
       </c>
@@ -1967,7 +2552,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>40737</v>
+      </c>
+      <c r="C99" t="s">
+        <v>259</v>
+      </c>
       <c r="D99" s="3" t="s">
         <v>101</v>
       </c>
@@ -1975,7 +2566,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>10942</v>
+      </c>
+      <c r="C100" t="s">
+        <v>259</v>
+      </c>
       <c r="D100" s="3" t="s">
         <v>102</v>
       </c>
@@ -1983,7 +2580,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>10943</v>
+      </c>
+      <c r="C101" t="s">
+        <v>259</v>
+      </c>
       <c r="D101" s="3" t="s">
         <v>103</v>
       </c>
@@ -1991,7 +2594,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>10964</v>
+      </c>
+      <c r="C102" t="s">
+        <v>259</v>
+      </c>
       <c r="D102" s="3" t="s">
         <v>104</v>
       </c>
@@ -1999,7 +2608,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>10979</v>
+      </c>
+      <c r="C103" t="s">
+        <v>259</v>
+      </c>
       <c r="D103" s="3" t="s">
         <v>105</v>
       </c>
@@ -2007,7 +2622,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>13420</v>
+      </c>
+      <c r="C104" t="s">
+        <v>259</v>
+      </c>
       <c r="D104" s="3" t="s">
         <v>106</v>
       </c>
@@ -2015,7 +2636,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>13421</v>
+      </c>
+      <c r="C105" t="s">
+        <v>259</v>
+      </c>
       <c r="D105" s="3" t="s">
         <v>107</v>
       </c>
@@ -2023,7 +2650,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>11299</v>
+      </c>
+      <c r="C106" t="s">
+        <v>259</v>
+      </c>
       <c r="D106" s="3" t="s">
         <v>108</v>
       </c>
@@ -2031,7 +2664,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>12671</v>
+      </c>
+      <c r="C107" t="s">
+        <v>259</v>
+      </c>
       <c r="D107" s="3" t="s">
         <v>109</v>
       </c>
@@ -2039,7 +2678,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>11023</v>
+      </c>
+      <c r="C108" t="s">
+        <v>259</v>
+      </c>
       <c r="D108" s="3" t="s">
         <v>110</v>
       </c>
@@ -2047,7 +2692,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>13229</v>
+      </c>
+      <c r="C109" t="s">
+        <v>259</v>
+      </c>
       <c r="D109" s="3" t="s">
         <v>111</v>
       </c>
@@ -2055,7 +2706,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>11031</v>
+      </c>
+      <c r="C110" t="s">
+        <v>259</v>
+      </c>
       <c r="D110" s="3" t="s">
         <v>112</v>
       </c>
@@ -2063,7 +2720,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>12152</v>
+      </c>
+      <c r="C111" t="s">
+        <v>259</v>
+      </c>
       <c r="D111" s="3" t="s">
         <v>113</v>
       </c>
@@ -2071,7 +2734,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>40810</v>
+      </c>
+      <c r="C112" t="s">
+        <v>259</v>
+      </c>
       <c r="D112" s="3" t="s">
         <v>114</v>
       </c>
@@ -2079,7 +2748,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>11065</v>
+      </c>
+      <c r="C113" t="s">
+        <v>259</v>
+      </c>
       <c r="D113" s="3" t="s">
         <v>115</v>
       </c>
@@ -2087,7 +2762,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>11089</v>
+      </c>
+      <c r="C114" t="s">
+        <v>259</v>
+      </c>
       <c r="D114" s="3" t="s">
         <v>116</v>
       </c>
@@ -2095,7 +2776,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>11121</v>
+      </c>
+      <c r="C115" t="s">
+        <v>259</v>
+      </c>
       <c r="D115" s="3" t="s">
         <v>117</v>
       </c>
@@ -2103,7 +2790,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>40630</v>
+      </c>
+      <c r="C116" t="s">
+        <v>259</v>
+      </c>
       <c r="D116" s="3" t="s">
         <v>118</v>
       </c>
@@ -2111,7 +2804,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>12207</v>
+      </c>
+      <c r="C117" t="s">
+        <v>259</v>
+      </c>
       <c r="D117" s="3" t="s">
         <v>119</v>
       </c>
@@ -2119,7 +2818,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>40732</v>
+      </c>
+      <c r="C118" t="s">
+        <v>259</v>
+      </c>
       <c r="D118" s="3" t="s">
         <v>120</v>
       </c>
@@ -2127,7 +2832,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>426</v>
+      </c>
+      <c r="C119" t="s">
+        <v>259</v>
+      </c>
       <c r="D119" s="3" t="s">
         <v>121</v>
       </c>
@@ -2135,7 +2846,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>12646</v>
+      </c>
+      <c r="C120" t="s">
+        <v>259</v>
+      </c>
       <c r="D120" s="3" t="s">
         <v>122</v>
       </c>
@@ -2143,7 +2860,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>13612</v>
+      </c>
+      <c r="C121" t="s">
+        <v>259</v>
+      </c>
       <c r="D121" s="3" t="s">
         <v>123</v>
       </c>
@@ -2151,7 +2874,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>11336</v>
+      </c>
+      <c r="C122" t="s">
+        <v>259</v>
+      </c>
       <c r="D122" s="3" t="s">
         <v>124</v>
       </c>
@@ -2159,7 +2888,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>13423</v>
+      </c>
+      <c r="C123" t="s">
+        <v>259</v>
+      </c>
       <c r="D123" s="3" t="s">
         <v>125</v>
       </c>
@@ -2167,7 +2902,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>40628</v>
+      </c>
+      <c r="C124" t="s">
+        <v>259</v>
+      </c>
       <c r="D124" s="3" t="s">
         <v>126</v>
       </c>
@@ -2175,7 +2916,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>11133</v>
+      </c>
+      <c r="C125" t="s">
+        <v>259</v>
+      </c>
       <c r="D125" s="3" t="s">
         <v>127</v>
       </c>
@@ -2183,7 +2930,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>12552</v>
+      </c>
+      <c r="C126" t="s">
+        <v>259</v>
+      </c>
       <c r="D126" s="3" t="s">
         <v>128</v>
       </c>
@@ -2191,7 +2944,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>40489</v>
+      </c>
+      <c r="C127" t="s">
+        <v>259</v>
+      </c>
       <c r="D127" s="3" t="s">
         <v>129</v>
       </c>
@@ -2199,7 +2958,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>13164</v>
+      </c>
+      <c r="C128" t="s">
+        <v>259</v>
+      </c>
       <c r="D128" s="3" t="s">
         <v>130</v>
       </c>
@@ -2207,7 +2972,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>12310</v>
+      </c>
+      <c r="C129" t="s">
+        <v>259</v>
+      </c>
       <c r="D129" s="3" t="s">
         <v>131</v>
       </c>
@@ -2215,7 +2986,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>11199</v>
+      </c>
+      <c r="C130" t="s">
+        <v>259</v>
+      </c>
       <c r="D130" s="3" t="s">
         <v>132</v>
       </c>
@@ -2223,7 +3000,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>11194</v>
+      </c>
+      <c r="C131" t="s">
+        <v>259</v>
+      </c>
       <c r="D131" s="3" t="s">
         <v>133</v>
       </c>
@@ -2231,7 +3014,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>12119</v>
+      </c>
+      <c r="C132" t="s">
+        <v>259</v>
+      </c>
       <c r="D132" s="3" t="s">
         <v>134</v>
       </c>
@@ -2239,7 +3028,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>11195</v>
+      </c>
+      <c r="C133" t="s">
+        <v>259</v>
+      </c>
       <c r="D133" s="3" t="s">
         <v>135</v>
       </c>
@@ -2247,7 +3042,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>13178</v>
+      </c>
+      <c r="C134" t="s">
+        <v>259</v>
+      </c>
       <c r="D134" s="3" t="s">
         <v>136</v>
       </c>
@@ -2255,7 +3056,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>11211</v>
+      </c>
+      <c r="C135" t="s">
+        <v>259</v>
+      </c>
       <c r="D135" s="3" t="s">
         <v>137</v>
       </c>
@@ -2263,7 +3070,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>11218</v>
+      </c>
+      <c r="C136" t="s">
+        <v>259</v>
+      </c>
       <c r="D136" s="3" t="s">
         <v>138</v>
       </c>
@@ -2271,7 +3084,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>40064</v>
+      </c>
+      <c r="C137" t="s">
+        <v>259</v>
+      </c>
       <c r="D137" s="3" t="s">
         <v>139</v>
       </c>
@@ -2279,7 +3098,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>13011</v>
+      </c>
+      <c r="C138" t="s">
+        <v>259</v>
+      </c>
       <c r="D138" s="3" t="s">
         <v>140</v>
       </c>
@@ -2287,7 +3112,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>12971</v>
+      </c>
+      <c r="C139" t="s">
+        <v>259</v>
+      </c>
       <c r="D139" s="3" t="s">
         <v>141</v>
       </c>
@@ -2295,7 +3126,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>13142</v>
+      </c>
+      <c r="C140" t="s">
+        <v>259</v>
+      </c>
       <c r="D140" s="3" t="s">
         <v>142</v>
       </c>
@@ -2303,7 +3140,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>11256</v>
+      </c>
+      <c r="C141" t="s">
+        <v>259</v>
+      </c>
       <c r="D141" s="3" t="s">
         <v>143</v>
       </c>
@@ -2311,7 +3154,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>146</v>
+      </c>
+      <c r="C142" t="s">
+        <v>259</v>
+      </c>
       <c r="D142" s="3" t="s">
         <v>144</v>
       </c>
@@ -2319,7 +3168,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="143" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>13162</v>
+      </c>
+      <c r="C143" t="s">
+        <v>259</v>
+      </c>
       <c r="D143" s="3" t="s">
         <v>145</v>
       </c>
@@ -2327,7 +3182,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="144" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>13722</v>
+      </c>
+      <c r="C144" t="s">
+        <v>259</v>
+      </c>
       <c r="D144" s="3" t="s">
         <v>14</v>
       </c>
@@ -2335,7 +3196,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>12126</v>
+      </c>
+      <c r="C145" t="s">
+        <v>259</v>
+      </c>
       <c r="D145" s="3" t="s">
         <v>146</v>
       </c>
@@ -2343,7 +3210,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>12103</v>
+      </c>
+      <c r="C146" t="s">
+        <v>259</v>
+      </c>
       <c r="D146" s="3" t="s">
         <v>147</v>
       </c>
@@ -2351,7 +3224,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>11482</v>
+      </c>
+      <c r="C147" t="s">
+        <v>259</v>
+      </c>
       <c r="D147" s="3" t="s">
         <v>148</v>
       </c>
@@ -2359,7 +3238,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="148" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>12520</v>
+      </c>
+      <c r="C148" t="s">
+        <v>259</v>
+      </c>
       <c r="D148" s="3" t="s">
         <v>149</v>
       </c>
@@ -2367,7 +3252,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="149" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>10508</v>
+      </c>
+      <c r="C149" t="s">
+        <v>259</v>
+      </c>
       <c r="D149" s="3" t="s">
         <v>23</v>
       </c>
@@ -2375,7 +3266,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>10503</v>
+      </c>
+      <c r="C150" t="s">
+        <v>259</v>
+      </c>
       <c r="D150" s="3" t="s">
         <v>150</v>
       </c>
@@ -2383,7 +3280,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>13520</v>
+      </c>
+      <c r="C151" t="s">
+        <v>259</v>
+      </c>
       <c r="D151" s="3" t="s">
         <v>151</v>
       </c>
@@ -2391,7 +3294,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="152" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>40856</v>
+      </c>
+      <c r="C152" t="s">
+        <v>259</v>
+      </c>
       <c r="D152" s="3" t="s">
         <v>152</v>
       </c>
@@ -2399,7 +3308,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="153" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>12904</v>
+      </c>
+      <c r="C153" t="s">
+        <v>259</v>
+      </c>
       <c r="D153" s="3" t="s">
         <v>153</v>
       </c>
@@ -2407,7 +3322,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="154" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>13219</v>
+      </c>
+      <c r="C154" t="s">
+        <v>259</v>
+      </c>
       <c r="D154" s="3" t="s">
         <v>154</v>
       </c>
@@ -2415,7 +3336,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="155" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>11609</v>
+      </c>
+      <c r="C155" t="s">
+        <v>259</v>
+      </c>
       <c r="D155" s="3" t="s">
         <v>155</v>
       </c>
@@ -2423,7 +3350,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="156" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>10560</v>
+      </c>
+      <c r="C156" t="s">
+        <v>259</v>
+      </c>
       <c r="D156" s="3" t="s">
         <v>41</v>
       </c>
@@ -2431,7 +3364,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="157" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>10583</v>
+      </c>
+      <c r="C157" t="s">
+        <v>259</v>
+      </c>
       <c r="D157" s="3" t="s">
         <v>156</v>
       </c>
@@ -2439,7 +3378,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="158" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>41111</v>
+      </c>
+      <c r="C158" t="s">
+        <v>259</v>
+      </c>
       <c r="D158" s="3" t="s">
         <v>157</v>
       </c>
@@ -2447,7 +3392,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="159" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>10567</v>
+      </c>
+      <c r="C159" t="s">
+        <v>259</v>
+      </c>
       <c r="D159" s="3" t="s">
         <v>8</v>
       </c>
@@ -2455,7 +3406,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="160" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>10588</v>
+      </c>
+      <c r="C160" t="s">
+        <v>259</v>
+      </c>
       <c r="D160" s="3" t="s">
         <v>158</v>
       </c>
@@ -2463,7 +3420,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="161" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>10606</v>
+      </c>
+      <c r="C161" t="s">
+        <v>259</v>
+      </c>
       <c r="D161" s="3" t="s">
         <v>48</v>
       </c>
@@ -2471,7 +3434,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="162" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>10591</v>
+      </c>
+      <c r="C162" t="s">
+        <v>259</v>
+      </c>
       <c r="D162" s="3" t="s">
         <v>49</v>
       </c>
@@ -2479,7 +3448,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="163" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>11562</v>
+      </c>
+      <c r="C163" t="s">
+        <v>259</v>
+      </c>
       <c r="D163" s="3" t="s">
         <v>159</v>
       </c>
@@ -2487,7 +3462,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="164" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>11007</v>
+      </c>
+      <c r="C164" t="s">
+        <v>259</v>
+      </c>
       <c r="D164" s="3" t="s">
         <v>160</v>
       </c>
@@ -2495,7 +3476,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="165" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>10611</v>
+      </c>
+      <c r="C165" t="s">
+        <v>259</v>
+      </c>
       <c r="D165" s="3" t="s">
         <v>161</v>
       </c>
@@ -2503,7 +3490,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="166" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>13555</v>
+      </c>
+      <c r="C166" t="s">
+        <v>259</v>
+      </c>
       <c r="D166" s="3" t="s">
         <v>162</v>
       </c>
@@ -2511,7 +3504,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="167" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>10624</v>
+      </c>
+      <c r="C167" t="s">
+        <v>259</v>
+      </c>
       <c r="D167" s="3" t="s">
         <v>163</v>
       </c>
@@ -2519,7 +3518,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="168" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>12027</v>
+      </c>
+      <c r="C168" t="s">
+        <v>259</v>
+      </c>
       <c r="D168" s="3" t="s">
         <v>164</v>
       </c>
@@ -2527,7 +3532,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="169" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>10643</v>
+      </c>
+      <c r="C169" t="s">
+        <v>259</v>
+      </c>
       <c r="D169" s="3" t="s">
         <v>165</v>
       </c>
@@ -2535,7 +3546,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="170" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>12140</v>
+      </c>
+      <c r="C170" t="s">
+        <v>259</v>
+      </c>
       <c r="D170" s="3" t="s">
         <v>166</v>
       </c>
@@ -2543,7 +3560,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="171" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>40888</v>
+      </c>
+      <c r="C171" t="s">
+        <v>259</v>
+      </c>
       <c r="D171" s="3" t="s">
         <v>167</v>
       </c>
@@ -2551,7 +3574,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="172" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>40461</v>
+      </c>
+      <c r="C172" t="s">
+        <v>259</v>
+      </c>
       <c r="D172" s="3" t="s">
         <v>168</v>
       </c>
@@ -2559,7 +3588,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="173" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>10672</v>
+      </c>
+      <c r="C173" t="s">
+        <v>259</v>
+      </c>
       <c r="D173" s="3" t="s">
         <v>169</v>
       </c>
@@ -2567,7 +3602,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="174" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>40309</v>
+      </c>
+      <c r="C174" t="s">
+        <v>259</v>
+      </c>
       <c r="D174" s="3" t="s">
         <v>170</v>
       </c>
@@ -2575,7 +3616,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="175" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>10680</v>
+      </c>
+      <c r="C175" t="s">
+        <v>259</v>
+      </c>
       <c r="D175" s="3" t="s">
         <v>171</v>
       </c>
@@ -2583,7 +3630,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="176" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>10610</v>
+      </c>
+      <c r="C176" t="s">
+        <v>259</v>
+      </c>
       <c r="D176" s="3" t="s">
         <v>172</v>
       </c>
@@ -2591,7 +3644,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>11556</v>
+      </c>
+      <c r="C177" t="s">
+        <v>259</v>
+      </c>
       <c r="D177" s="3" t="s">
         <v>173</v>
       </c>
@@ -2599,7 +3658,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>41055</v>
+      </c>
+      <c r="C178" t="s">
+        <v>259</v>
+      </c>
       <c r="D178" s="3" t="s">
         <v>174</v>
       </c>
@@ -2607,7 +3672,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>12571</v>
+      </c>
+      <c r="C179" t="s">
+        <v>259</v>
+      </c>
       <c r="D179" s="3" t="s">
         <v>175</v>
       </c>
@@ -2615,7 +3686,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="180" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>12024</v>
+      </c>
+      <c r="C180" t="s">
+        <v>259</v>
+      </c>
       <c r="D180" s="3" t="s">
         <v>176</v>
       </c>
@@ -2623,7 +3700,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>11757</v>
+      </c>
+      <c r="C181" t="s">
+        <v>259</v>
+      </c>
       <c r="D181" s="3" t="s">
         <v>177</v>
       </c>
@@ -2631,7 +3714,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>10726</v>
+      </c>
+      <c r="C182" t="s">
+        <v>259</v>
+      </c>
       <c r="D182" s="3" t="s">
         <v>178</v>
       </c>
@@ -2639,7 +3728,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="183" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>12961</v>
+      </c>
+      <c r="C183" t="s">
+        <v>259</v>
+      </c>
       <c r="D183" s="3" t="s">
         <v>179</v>
       </c>
@@ -2647,7 +3742,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="184" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>12955</v>
+      </c>
+      <c r="C184" t="s">
+        <v>259</v>
+      </c>
       <c r="D184" s="3" t="s">
         <v>180</v>
       </c>
@@ -2655,7 +3756,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="185" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>10745</v>
+      </c>
+      <c r="C185" t="s">
+        <v>259</v>
+      </c>
       <c r="D185" s="3" t="s">
         <v>181</v>
       </c>
@@ -2663,7 +3770,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="186" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>40176</v>
+      </c>
+      <c r="C186" t="s">
+        <v>259</v>
+      </c>
       <c r="D186" s="3" t="s">
         <v>182</v>
       </c>
@@ -2671,7 +3784,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="187" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>12979</v>
+      </c>
+      <c r="C187" t="s">
+        <v>259</v>
+      </c>
       <c r="D187" s="3" t="s">
         <v>183</v>
       </c>
@@ -2679,7 +3798,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="188" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>12124</v>
+      </c>
+      <c r="C188" t="s">
+        <v>259</v>
+      </c>
       <c r="D188" s="3" t="s">
         <v>63</v>
       </c>
@@ -2687,7 +3812,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="189" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>40636</v>
+      </c>
+      <c r="C189" t="s">
+        <v>259</v>
+      </c>
       <c r="D189" s="3" t="s">
         <v>184</v>
       </c>
@@ -2695,7 +3826,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="190" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>40979</v>
+      </c>
+      <c r="C190" t="s">
+        <v>259</v>
+      </c>
       <c r="D190" s="3" t="s">
         <v>185</v>
       </c>
@@ -2703,7 +3840,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="191" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>41042</v>
+      </c>
+      <c r="C191" t="s">
+        <v>259</v>
+      </c>
       <c r="D191" s="3" t="s">
         <v>65</v>
       </c>
@@ -2711,7 +3854,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="192" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>40889</v>
+      </c>
+      <c r="C192" t="s">
+        <v>259</v>
+      </c>
       <c r="D192" s="3" t="s">
         <v>186</v>
       </c>
@@ -2719,7 +3868,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="193" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>40321</v>
+      </c>
+      <c r="C193" t="s">
+        <v>259</v>
+      </c>
       <c r="D193" s="3" t="s">
         <v>187</v>
       </c>
@@ -2727,7 +3882,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="194" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>11407</v>
+      </c>
+      <c r="C194" t="s">
+        <v>259</v>
+      </c>
       <c r="D194" s="3" t="s">
         <v>188</v>
       </c>
@@ -2735,7 +3896,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="195" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>10761</v>
+      </c>
+      <c r="C195" t="s">
+        <v>259</v>
+      </c>
       <c r="D195" s="3" t="s">
         <v>189</v>
       </c>
@@ -2743,7 +3910,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="196" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>12449</v>
+      </c>
+      <c r="C196" t="s">
+        <v>259</v>
+      </c>
       <c r="D196" s="3" t="s">
         <v>190</v>
       </c>
@@ -2751,7 +3924,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="197" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>12451</v>
+      </c>
+      <c r="C197" t="s">
+        <v>259</v>
+      </c>
       <c r="D197" s="3" t="s">
         <v>191</v>
       </c>
@@ -2759,7 +3938,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="198" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>10835</v>
+      </c>
+      <c r="C198" t="s">
+        <v>259</v>
+      </c>
       <c r="D198" s="3" t="s">
         <v>192</v>
       </c>
@@ -2767,7 +3952,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="199" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>10805</v>
+      </c>
+      <c r="C199" t="s">
+        <v>259</v>
+      </c>
       <c r="D199" s="3" t="s">
         <v>193</v>
       </c>
@@ -2775,7 +3966,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="200" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>10816</v>
+      </c>
+      <c r="C200" t="s">
+        <v>259</v>
+      </c>
       <c r="D200" s="3" t="s">
         <v>194</v>
       </c>
@@ -2783,7 +3980,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>10814</v>
+      </c>
+      <c r="C201" t="s">
+        <v>259</v>
+      </c>
       <c r="D201" s="3" t="s">
         <v>195</v>
       </c>
@@ -2791,7 +3994,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="202" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>10551</v>
+      </c>
+      <c r="C202" t="s">
+        <v>259</v>
+      </c>
       <c r="D202" s="3" t="s">
         <v>196</v>
       </c>
@@ -2799,7 +4008,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="203" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>10826</v>
+      </c>
+      <c r="C203" t="s">
+        <v>259</v>
+      </c>
       <c r="D203" s="3" t="s">
         <v>81</v>
       </c>
@@ -2807,7 +4022,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="204" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>11366</v>
+      </c>
+      <c r="C204" t="s">
+        <v>259</v>
+      </c>
       <c r="D204" s="3" t="s">
         <v>197</v>
       </c>
@@ -2815,7 +4036,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>40853</v>
+      </c>
+      <c r="C205" t="s">
+        <v>259</v>
+      </c>
       <c r="D205" s="3" t="s">
         <v>198</v>
       </c>
@@ -2823,7 +4050,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="206" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>10900</v>
+      </c>
+      <c r="C206" t="s">
+        <v>259</v>
+      </c>
       <c r="D206" s="3" t="s">
         <v>84</v>
       </c>
@@ -2831,7 +4064,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="207" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>11292</v>
+      </c>
+      <c r="C207" t="s">
+        <v>259</v>
+      </c>
       <c r="D207" s="3" t="s">
         <v>199</v>
       </c>
@@ -2839,7 +4078,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="208" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>10897</v>
+      </c>
+      <c r="C208" t="s">
+        <v>259</v>
+      </c>
       <c r="D208" s="3" t="s">
         <v>91</v>
       </c>
@@ -2847,7 +4092,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="209" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>40320</v>
+      </c>
+      <c r="C209" t="s">
+        <v>259</v>
+      </c>
       <c r="D209" s="3" t="s">
         <v>200</v>
       </c>
@@ -2855,7 +4106,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="210" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>41018</v>
+      </c>
+      <c r="C210" t="s">
+        <v>259</v>
+      </c>
       <c r="D210" s="3" t="s">
         <v>201</v>
       </c>
@@ -2863,7 +4120,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="211" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>12122</v>
+      </c>
+      <c r="C211" t="s">
+        <v>259</v>
+      </c>
       <c r="D211" s="3" t="s">
         <v>202</v>
       </c>
@@ -2871,7 +4134,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="212" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>10997</v>
+      </c>
+      <c r="C212" t="s">
+        <v>259</v>
+      </c>
       <c r="D212" s="3" t="s">
         <v>203</v>
       </c>
@@ -2879,7 +4148,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="213" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>11457</v>
+      </c>
+      <c r="C213" t="s">
+        <v>259</v>
+      </c>
       <c r="D213" s="3" t="s">
         <v>204</v>
       </c>
@@ -2887,7 +4162,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="214" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>10919</v>
+      </c>
+      <c r="C214" t="s">
+        <v>259</v>
+      </c>
       <c r="D214" s="3" t="s">
         <v>94</v>
       </c>
@@ -2895,7 +4176,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="215" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>40101</v>
+      </c>
+      <c r="C215" t="s">
+        <v>259</v>
+      </c>
       <c r="D215" s="3" t="s">
         <v>205</v>
       </c>
@@ -2903,7 +4190,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="216" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>11896</v>
+      </c>
+      <c r="C216" t="s">
+        <v>259</v>
+      </c>
       <c r="D216" s="3" t="s">
         <v>97</v>
       </c>
@@ -2911,7 +4204,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="217" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>40737</v>
+      </c>
+      <c r="C217" t="s">
+        <v>259</v>
+      </c>
       <c r="D217" s="3" t="s">
         <v>101</v>
       </c>
@@ -2919,7 +4218,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="218" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>40615</v>
+      </c>
+      <c r="C218" t="s">
+        <v>259</v>
+      </c>
       <c r="D218" s="3" t="s">
         <v>206</v>
       </c>
@@ -2927,7 +4232,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="219" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>10943</v>
+      </c>
+      <c r="C219" t="s">
+        <v>259</v>
+      </c>
       <c r="D219" s="3" t="s">
         <v>103</v>
       </c>
@@ -2935,7 +4246,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="220" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>40839</v>
+      </c>
+      <c r="C220" t="s">
+        <v>259</v>
+      </c>
       <c r="D220" s="3" t="s">
         <v>207</v>
       </c>
@@ -2943,7 +4260,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="221" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>10963</v>
+      </c>
+      <c r="C221" t="s">
+        <v>259</v>
+      </c>
       <c r="D221" s="3" t="s">
         <v>208</v>
       </c>
@@ -2951,7 +4274,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="222" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>11747</v>
+      </c>
+      <c r="C222" t="s">
+        <v>259</v>
+      </c>
       <c r="D222" s="3" t="s">
         <v>209</v>
       </c>
@@ -2959,7 +4288,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="223" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>40483</v>
+      </c>
+      <c r="C223" t="s">
+        <v>259</v>
+      </c>
       <c r="D223" s="3" t="s">
         <v>210</v>
       </c>
@@ -2967,7 +4302,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="224" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>10982</v>
+      </c>
+      <c r="C224" t="s">
+        <v>259</v>
+      </c>
       <c r="D224" s="3" t="s">
         <v>211</v>
       </c>
@@ -2975,7 +4316,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>12612</v>
+      </c>
+      <c r="C225" t="s">
+        <v>259</v>
+      </c>
       <c r="D225" s="3" t="s">
         <v>212</v>
       </c>
@@ -2983,7 +4330,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>12076</v>
+      </c>
+      <c r="C226" t="s">
+        <v>259</v>
+      </c>
       <c r="D226" s="3" t="s">
         <v>213</v>
       </c>
@@ -2991,7 +4344,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>40504</v>
+      </c>
+      <c r="C227" t="s">
+        <v>259</v>
+      </c>
       <c r="D227" s="3" t="s">
         <v>214</v>
       </c>
@@ -2999,7 +4358,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>10991</v>
+      </c>
+      <c r="C228" t="s">
+        <v>259</v>
+      </c>
       <c r="D228" s="3" t="s">
         <v>215</v>
       </c>
@@ -3007,7 +4372,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>12459</v>
+      </c>
+      <c r="C229" t="s">
+        <v>259</v>
+      </c>
       <c r="D229" s="3" t="s">
         <v>216</v>
       </c>
@@ -3015,7 +4386,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>40152</v>
+      </c>
+      <c r="C230" t="s">
+        <v>259</v>
+      </c>
       <c r="D230" s="3" t="s">
         <v>217</v>
       </c>
@@ -3023,7 +4400,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>12671</v>
+      </c>
+      <c r="C231" t="s">
+        <v>259</v>
+      </c>
       <c r="D231" s="3" t="s">
         <v>109</v>
       </c>
@@ -3031,7 +4414,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>11089</v>
+      </c>
+      <c r="C232" t="s">
+        <v>259</v>
+      </c>
       <c r="D232" s="3" t="s">
         <v>116</v>
       </c>
@@ -3039,7 +4428,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>40926</v>
+      </c>
+      <c r="C233" t="s">
+        <v>259</v>
+      </c>
       <c r="D233" s="3" t="s">
         <v>218</v>
       </c>
@@ -3047,7 +4442,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>10202</v>
+      </c>
+      <c r="C234" t="s">
+        <v>259</v>
+      </c>
       <c r="D234" s="3" t="s">
         <v>219</v>
       </c>
@@ -3055,7 +4456,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>11109</v>
+      </c>
+      <c r="C235" t="s">
+        <v>259</v>
+      </c>
       <c r="D235" s="3" t="s">
         <v>220</v>
       </c>
@@ -3063,7 +4470,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>11111</v>
+      </c>
+      <c r="C236" t="s">
+        <v>259</v>
+      </c>
       <c r="D236" s="3" t="s">
         <v>221</v>
       </c>
@@ -3071,7 +4484,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>11126</v>
+      </c>
+      <c r="C237" t="s">
+        <v>259</v>
+      </c>
       <c r="D237" s="3" t="s">
         <v>222</v>
       </c>
@@ -3079,7 +4498,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>13612</v>
+      </c>
+      <c r="C238" t="s">
+        <v>259</v>
+      </c>
       <c r="D238" s="3" t="s">
         <v>123</v>
       </c>
@@ -3087,7 +4512,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>11127</v>
+      </c>
+      <c r="C239" t="s">
+        <v>259</v>
+      </c>
       <c r="D239" s="3" t="s">
         <v>223</v>
       </c>
@@ -3095,7 +4526,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>12109</v>
+      </c>
+      <c r="C240" t="s">
+        <v>259</v>
+      </c>
       <c r="D240" s="3" t="s">
         <v>224</v>
       </c>
@@ -3103,7 +4540,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="241" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>11616</v>
+      </c>
+      <c r="C241" t="s">
+        <v>259</v>
+      </c>
       <c r="D241" s="3" t="s">
         <v>225</v>
       </c>
@@ -3111,7 +4554,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="242" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>41030</v>
+      </c>
+      <c r="C242" t="s">
+        <v>259</v>
+      </c>
       <c r="D242" s="3" t="s">
         <v>226</v>
       </c>
@@ -3119,7 +4568,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="243" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>11135</v>
+      </c>
+      <c r="C243" t="s">
+        <v>259</v>
+      </c>
       <c r="D243" s="3" t="s">
         <v>227</v>
       </c>
@@ -3127,7 +4582,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="244" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>11136</v>
+      </c>
+      <c r="C244" t="s">
+        <v>259</v>
+      </c>
       <c r="D244" s="3" t="s">
         <v>228</v>
       </c>
@@ -3135,7 +4596,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="245" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>11158</v>
+      </c>
+      <c r="C245" t="s">
+        <v>259</v>
+      </c>
       <c r="D245" s="3" t="s">
         <v>229</v>
       </c>
@@ -3143,7 +4610,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="246" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>40489</v>
+      </c>
+      <c r="C246" t="s">
+        <v>259</v>
+      </c>
       <c r="D246" s="3" t="s">
         <v>129</v>
       </c>
@@ -3151,7 +4624,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="247" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>11150</v>
+      </c>
+      <c r="C247" t="s">
+        <v>259</v>
+      </c>
       <c r="D247" s="3" t="s">
         <v>230</v>
       </c>
@@ -3159,7 +4638,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="248" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>13644</v>
+      </c>
+      <c r="C248" t="s">
+        <v>259</v>
+      </c>
       <c r="D248" s="3" t="s">
         <v>231</v>
       </c>
@@ -3167,7 +4652,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="249" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>11873</v>
+      </c>
+      <c r="C249" t="s">
+        <v>259</v>
+      </c>
       <c r="D249" s="3" t="s">
         <v>232</v>
       </c>
@@ -3175,7 +4666,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="250" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>40744</v>
+      </c>
+      <c r="C250" t="s">
+        <v>259</v>
+      </c>
       <c r="D250" s="3" t="s">
         <v>233</v>
       </c>
@@ -3183,7 +4680,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="251" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>13178</v>
+      </c>
+      <c r="C251" t="s">
+        <v>259</v>
+      </c>
       <c r="D251" s="3" t="s">
         <v>136</v>
       </c>
@@ -3191,7 +4694,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="252" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>11205</v>
+      </c>
+      <c r="C252" t="s">
+        <v>259</v>
+      </c>
       <c r="D252" s="3" t="s">
         <v>234</v>
       </c>
@@ -3199,7 +4708,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="253" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>13278</v>
+      </c>
+      <c r="C253" t="s">
+        <v>259</v>
+      </c>
       <c r="D253" s="3" t="s">
         <v>235</v>
       </c>
@@ -3207,7 +4722,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="254" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>12115</v>
+      </c>
+      <c r="C254" t="s">
+        <v>259</v>
+      </c>
       <c r="D254" s="3" t="s">
         <v>236</v>
       </c>
@@ -3215,7 +4736,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="255" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>12054</v>
+      </c>
+      <c r="C255" t="s">
+        <v>259</v>
+      </c>
       <c r="D255" s="3" t="s">
         <v>237</v>
       </c>
@@ -3223,7 +4750,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="256" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>12592</v>
+      </c>
+      <c r="C256" t="s">
+        <v>259</v>
+      </c>
       <c r="D256" s="3" t="s">
         <v>238</v>
       </c>
@@ -3231,7 +4764,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>41059</v>
+      </c>
+      <c r="C257" t="s">
+        <v>259</v>
+      </c>
       <c r="D257" s="3" t="s">
         <v>239</v>
       </c>
@@ -3239,7 +4778,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <v>11506</v>
+      </c>
+      <c r="C258" t="s">
+        <v>259</v>
+      </c>
       <c r="D258" s="3" t="s">
         <v>240</v>
       </c>
@@ -3247,7 +4792,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>12116</v>
+      </c>
+      <c r="C259" t="s">
+        <v>259</v>
+      </c>
       <c r="D259" s="3" t="s">
         <v>241</v>
       </c>
@@ -3255,7 +4806,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="260" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>11212</v>
+      </c>
+      <c r="C260" t="s">
+        <v>259</v>
+      </c>
       <c r="D260" s="3" t="s">
         <v>242</v>
       </c>
@@ -3263,7 +4820,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="261" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>11213</v>
+      </c>
+      <c r="C261" t="s">
+        <v>259</v>
+      </c>
       <c r="D261" s="3" t="s">
         <v>243</v>
       </c>
@@ -3271,7 +4834,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="262" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <v>12108</v>
+      </c>
+      <c r="C262" t="s">
+        <v>259</v>
+      </c>
       <c r="D262" s="3" t="s">
         <v>244</v>
       </c>
@@ -3279,7 +4848,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="263" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B263">
+        <v>40711</v>
+      </c>
+      <c r="C263" t="s">
+        <v>259</v>
+      </c>
       <c r="D263" s="3" t="s">
         <v>245</v>
       </c>
@@ -3287,7 +4862,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="264" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B264">
+        <v>12114</v>
+      </c>
+      <c r="C264" t="s">
+        <v>259</v>
+      </c>
       <c r="D264" s="3" t="s">
         <v>246</v>
       </c>
@@ -3295,7 +4876,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="265" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B265">
+        <v>11256</v>
+      </c>
+      <c r="C265" t="s">
+        <v>259</v>
+      </c>
       <c r="D265" s="3" t="s">
         <v>143</v>
       </c>
@@ -3303,7 +4890,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="266" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B266">
+        <v>12603</v>
+      </c>
+      <c r="C266" t="s">
+        <v>259</v>
+      </c>
       <c r="D266" s="3" t="s">
         <v>247</v>
       </c>
@@ -3311,7 +4904,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="267" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B267">
+        <v>12117</v>
+      </c>
+      <c r="C267" t="s">
+        <v>259</v>
+      </c>
       <c r="D267" s="3" t="s">
         <v>248</v>
       </c>
@@ -3319,7 +4918,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="268" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B268">
+        <v>12501</v>
+      </c>
+      <c r="C268" t="s">
+        <v>259</v>
+      </c>
       <c r="D268" s="3" t="s">
         <v>249</v>
       </c>
@@ -3327,7 +4932,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="269" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <v>12118</v>
+      </c>
+      <c r="C269" t="s">
+        <v>259</v>
+      </c>
       <c r="D269" s="3" t="s">
         <v>250</v>
       </c>
@@ -3335,7 +4946,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="270" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B270">
+        <v>12399</v>
+      </c>
+      <c r="C270" t="s">
+        <v>259</v>
+      </c>
       <c r="D270" s="3" t="s">
         <v>251</v>
       </c>
@@ -3343,7 +4960,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="271" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B271">
+        <v>35834</v>
+      </c>
+      <c r="C271" t="s">
+        <v>259</v>
+      </c>
       <c r="D271" s="3" t="s">
         <v>252</v>
       </c>
@@ -3351,7 +4974,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="272" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B272">
+        <v>391</v>
+      </c>
+      <c r="C272" t="s">
+        <v>259</v>
+      </c>
       <c r="D272" s="3" t="s">
         <v>253</v>
       </c>
@@ -3359,7 +4988,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="273" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>12286</v>
+      </c>
+      <c r="C273" t="s">
+        <v>259</v>
+      </c>
       <c r="D273" s="3" t="s">
         <v>254</v>
       </c>
@@ -3367,7 +5002,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="274" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <v>11614</v>
+      </c>
+      <c r="C274" t="s">
+        <v>259</v>
+      </c>
       <c r="D274" s="3" t="s">
         <v>255</v>
       </c>

</xml_diff>